<commit_message>
postgame pitcher reports done!
</commit_message>
<xml_diff>
--- a/postgame_pitcher_reports/COR_KNI/2022-07-29/Brotherton, Duke.xlsx
+++ b/postgame_pitcher_reports/COR_KNI/2022-07-29/Brotherton, Duke.xlsx
@@ -1537,6 +1537,186 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>9</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>24</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>39</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>54</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>69</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>90</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>2</col>
+      <colOff>0</colOff>
+      <row>105</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1457325" cy="1914525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6594,5 +6774,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="89" min="1" max="13" man="1"/>
   </rowBreaks>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>